<commit_message>
fixed deriva compounds_props, add iupac to cal
</commit_message>
<xml_diff>
--- a/tests/data_for_testing/compounds_properties.xlsx
+++ b/tests/data_for_testing/compounds_properties.xlsx
@@ -593,56 +593,56 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>tetradecanoic acid</t>
+          <t>oleic acid</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>tetradecanoic acid</t>
+          <t>(z)-octadec-9-enoic acid</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C14H28O2</t>
+          <t>C18H34O2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCC(=O)O</t>
+          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>228.37</v>
+        <v>282.5</v>
       </c>
       <c r="F2" t="n">
-        <v>5.3</v>
+        <v>6.5</v>
       </c>
       <c r="G2" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J2" t="n">
         <v>2</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7363226343214958</v>
+        <v>0.7653026548672566</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1235889127293427</v>
+        <v>0.121316814159292</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1401147261023777</v>
+        <v>0.1132672566371681</v>
       </c>
       <c r="O2" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -666,7 +666,7 @@
         <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>0.8029031834303979</v>
+        <v>0.8405345132743363</v>
       </c>
       <c r="X2" t="n">
         <v>0</v>
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.1971230897228183</v>
+        <v>0.1593522123893805</v>
       </c>
       <c r="AB2" t="n">
         <v>0</v>
@@ -690,62 +690,62 @@
         <v>0</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>oxacycloheptadecan-2-one</t>
+          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>oxacycloheptadecan-2-one</t>
+          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C16H30O2</t>
+          <t>C18H32O2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>C1CCCCCCCC(=O)OCCCCCCC1</t>
+          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>254.41</v>
+        <v>280.4</v>
       </c>
       <c r="F3" t="n">
-        <v>6.3</v>
+        <v>6.8</v>
       </c>
       <c r="G3" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J3" t="n">
         <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7553791124562713</v>
+        <v>0.7710342368045648</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.1188632522306513</v>
+        <v>0.1150356633380885</v>
       </c>
       <c r="N3" t="n">
-        <v>0.1257733579654888</v>
+        <v>0.1141155492154066</v>
       </c>
       <c r="O3" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="P3" t="n">
         <v>0</v>
@@ -757,10 +757,10 @@
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U3" t="n">
         <v>0</v>
@@ -769,7 +769,7 @@
         <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>0.771895758814512</v>
+        <v>0.8396398002853066</v>
       </c>
       <c r="X3" t="n">
         <v>0</v>
@@ -781,10 +781,10 @@
         <v>0</v>
       </c>
       <c r="AA3" t="n">
-        <v>0</v>
+        <v>0.1605456490727532</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.2281199638378994</v>
+        <v>0</v>
       </c>
       <c r="AC3" t="n">
         <v>0</v>
@@ -793,62 +793,62 @@
         <v>0</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>n-hexadecanoic acid</t>
+          <t>2,5-hexanedione</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>hexadecanoic acid</t>
+          <t>hexane-2,5-dione</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C16H32O2</t>
+          <t>C6H10O2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCCCC(=O)O</t>
+          <t>CC(=O)CCC(=O)C</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>256.42</v>
+        <v>114.14</v>
       </c>
       <c r="F4" t="n">
-        <v>6.4</v>
+        <v>-0.3</v>
       </c>
       <c r="G4" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="J4" t="n">
         <v>2</v>
       </c>
       <c r="K4" t="n">
-        <v>0.7494579205990172</v>
+        <v>0.6313825127036973</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.125793619842446</v>
+        <v>0.08831259856316805</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1247874580765931</v>
+        <v>0.2803399334151043</v>
       </c>
       <c r="O4" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
@@ -860,7 +860,7 @@
         <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4" t="n">
         <v>0</v>
@@ -869,10 +869,10 @@
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W4" t="n">
-        <v>0.8244793697839481</v>
+        <v>0</v>
       </c>
       <c r="X4" t="n">
         <v>0</v>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.1755596287341081</v>
+        <v>0</v>
       </c>
       <c r="AB4" t="n">
         <v>0</v>
@@ -893,65 +893,65 @@
         <v>0</v>
       </c>
       <c r="AD4" t="n">
-        <v>0</v>
+        <v>1.000035044681969</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>9,12-octadecadienoic acid (z,z)-</t>
+          <t>2-methylcyclopent-2-en-1-one</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
+          <t>2-methylcyclopent-2-en-1-one</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>C18H32O2</t>
+          <t>C6H8O</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
+          <t>CC1=CCCC1=O</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>280.4</v>
+        <v>96.13</v>
       </c>
       <c r="F5" t="n">
-        <v>6.8</v>
+        <v>0.9</v>
       </c>
       <c r="G5" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="J5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>0.7710342368045648</v>
+        <v>0.7496723187350464</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1150356633380885</v>
+        <v>0.08388640382814938</v>
       </c>
       <c r="N5" t="n">
-        <v>0.1141155492154066</v>
+        <v>0.1664308748569645</v>
       </c>
       <c r="O5" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="P5" t="n">
         <v>0</v>
@@ -963,19 +963,19 @@
         <v>0</v>
       </c>
       <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
         <v>1</v>
       </c>
-      <c r="T5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0</v>
-      </c>
       <c r="W5" t="n">
-        <v>0.8396398002853066</v>
+        <v>0.4377509622386352</v>
       </c>
       <c r="X5" t="n">
         <v>0</v>
@@ -987,7 +987,7 @@
         <v>0</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.1605456490727532</v>
+        <v>0</v>
       </c>
       <c r="AB5" t="n">
         <v>0</v>
@@ -996,168 +996,168 @@
         <v>0</v>
       </c>
       <c r="AD5" t="n">
-        <v>0</v>
+        <v>0.5936960366170811</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>oleic acid</t>
+          <t>2,4,5-trichlorophenol</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>(z)-octadec-9-enoic acid</t>
+          <t>2,4,5-trichlorophenol</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C18H34O2</t>
+          <t>C6H3Cl3O</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
+          <t>C1=C(C(=CC(=C1Cl)Cl)Cl)O</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>282.5</v>
+        <v>197.4</v>
       </c>
       <c r="F6" t="n">
-        <v>6.5</v>
+        <v>3.7</v>
       </c>
       <c r="G6" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I6" t="n">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="J6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>0.7653026548672566</v>
+        <v>0.3650759878419453</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>0.5387537993920973</v>
       </c>
       <c r="M6" t="n">
-        <v>0.121316814159292</v>
+        <v>0.01531914893617021</v>
       </c>
       <c r="N6" t="n">
-        <v>0.1132672566371681</v>
+        <v>0.08104863221884498</v>
       </c>
       <c r="O6" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6" t="n">
         <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V6" t="n">
         <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>0.8405345132743363</v>
+        <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>0</v>
+        <v>0.3752887537993921</v>
       </c>
       <c r="Y6" t="n">
-        <v>0</v>
+        <v>0.5387537993920973</v>
       </c>
       <c r="Z6" t="n">
-        <v>0</v>
+        <v>0.08615501519756839</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.1593522123893805</v>
+        <v>0</v>
       </c>
       <c r="AB6" t="n">
         <v>0</v>
       </c>
       <c r="AC6" t="n">
-        <v>0</v>
+        <v>0.5387537993920973</v>
       </c>
       <c r="AD6" t="n">
         <v>0</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>n-decanoic acid</t>
+          <t>9,12-octadecadienoic acid (z,z)-</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>decanoic acid</t>
+          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>C10H20O2</t>
+          <t>C18H32O2</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CCCCCCCCCC(=O)O</t>
+          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>172.26</v>
+        <v>280.4</v>
       </c>
       <c r="F7" t="n">
-        <v>4.1</v>
+        <v>6.8</v>
       </c>
       <c r="G7" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="J7" t="n">
         <v>2</v>
       </c>
       <c r="K7" t="n">
-        <v>0.6972599558806455</v>
+        <v>0.7710342368045648</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1170323928944619</v>
+        <v>0.1150356633380885</v>
       </c>
       <c r="N7" t="n">
-        <v>0.1857540926506444</v>
+        <v>0.1141155492154066</v>
       </c>
       <c r="O7" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
@@ -1181,7 +1181,7 @@
         <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>0.7387147335423198</v>
+        <v>0.8396398002853066</v>
       </c>
       <c r="X7" t="n">
         <v>0</v>
@@ -1193,7 +1193,7 @@
         <v>0</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.2613317078834321</v>
+        <v>0.1605456490727532</v>
       </c>
       <c r="AB7" t="n">
         <v>0</v>
@@ -1205,75 +1205,75 @@
         <v>0</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>2-butanone</t>
+          <t>tetradecanoic acid</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>butan-2-one</t>
+          <t>tetradecanoic acid</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C4H8O</t>
+          <t>C14H28O2</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CCC(=O)C</t>
+          <t>CCCCCCCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>72.11</v>
+        <v>228.37</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3</v>
+        <v>5.3</v>
       </c>
       <c r="G8" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="J8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.7363226343214958</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.1235889127293427</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.1401147261023777</v>
+      </c>
+      <c r="O8" t="n">
+        <v>13</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
         <v>1</v>
       </c>
-      <c r="K8" t="n">
-        <v>0.6662598807377618</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.1118291499098599</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.2218693662460131</v>
-      </c>
-      <c r="O8" t="n">
-        <v>1</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0</v>
-      </c>
       <c r="T8" t="n">
         <v>0</v>
       </c>
@@ -1281,10 +1281,10 @@
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>0.2085009014006379</v>
+        <v>0.8029031834303979</v>
       </c>
       <c r="X8" t="n">
         <v>0</v>
@@ -1296,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="AA8" t="n">
-        <v>0</v>
+        <v>0.1971230897228183</v>
       </c>
       <c r="AB8" t="n">
         <v>0</v>
@@ -1305,38 +1305,38 @@
         <v>0</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.7914574954929968</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>2-cyclopenten-1-one, 2-methyl-</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2-methylcyclopent-2-en-1-one</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>C6H8O</t>
+          <t>C6H6O</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>CC1=CCCC1=O</t>
+          <t>C1=CC=C(C=C1)O</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>96.13</v>
+        <v>94.11</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9</v>
+        <v>1.5</v>
       </c>
       <c r="G9" t="n">
         <v>6</v>
@@ -1345,34 +1345,34 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J9" t="n">
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>0.7496723187350464</v>
+        <v>0.765763468281798</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.08388640382814938</v>
+        <v>0.06426522154925088</v>
       </c>
       <c r="N9" t="n">
-        <v>0.1664308748569645</v>
+        <v>0.1700031877590054</v>
       </c>
       <c r="O9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q9" t="n">
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
@@ -1384,19 +1384,19 @@
         <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9" t="n">
-        <v>0.4377509622386352</v>
+        <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>0</v>
+        <v>0.8193178195728402</v>
       </c>
       <c r="Y9" t="n">
         <v>0</v>
       </c>
       <c r="Z9" t="n">
-        <v>0</v>
+        <v>0.1807140580172139</v>
       </c>
       <c r="AA9" t="n">
         <v>0</v>
@@ -1408,41 +1408,41 @@
         <v>0</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.5936960366170811</v>
+        <v>0</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>trans-2-pentenoic acid</t>
+          <t>2-butanone</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>(e)-pent-2-enoic acid</t>
+          <t>butan-2-one</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>C5H8O2</t>
+          <t>C4H8O</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>CCC=CC(=O)O</t>
+          <t>CCC(=O)C</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>100.12</v>
+        <v>72.11</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="G10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1451,22 +1451,22 @@
         <v>8</v>
       </c>
       <c r="J10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0.5998302037554933</v>
+        <v>0.6662598807377618</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>0.08054334798242109</v>
+        <v>0.1118291499098599</v>
       </c>
       <c r="N10" t="n">
-        <v>0.3195964842189373</v>
+        <v>0.2218693662460131</v>
       </c>
       <c r="O10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P10" t="n">
         <v>0</v>
@@ -1478,19 +1478,19 @@
         <v>0</v>
       </c>
       <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" t="n">
         <v>1</v>
       </c>
-      <c r="T10" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" t="n">
-        <v>0</v>
-      </c>
-      <c r="V10" t="n">
-        <v>0</v>
-      </c>
       <c r="W10" t="n">
-        <v>0.5503395924890131</v>
+        <v>0.2085009014006379</v>
       </c>
       <c r="X10" t="n">
         <v>0</v>
@@ -1502,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.4496304434678386</v>
+        <v>0</v>
       </c>
       <c r="AB10" t="n">
         <v>0</v>
@@ -1511,65 +1511,65 @@
         <v>0</v>
       </c>
       <c r="AD10" t="n">
-        <v>0</v>
+        <v>0.7914574954929968</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>2,5-hexanedione</t>
+          <t>(z)-octadec-9-enoic acid</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>hexane-2,5-dione</t>
+          <t>(z)-octadec-9-enoic acid</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>C6H10O2</t>
+          <t>C18H34O2</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CC(=O)CCC(=O)C</t>
+          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>114.14</v>
+        <v>282.5</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.3</v>
+        <v>6.5</v>
       </c>
       <c r="G11" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="J11" t="n">
         <v>2</v>
       </c>
       <c r="K11" t="n">
-        <v>0.6313825127036973</v>
+        <v>0.7653026548672566</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>0.08831259856316805</v>
+        <v>0.121316814159292</v>
       </c>
       <c r="N11" t="n">
-        <v>0.2803399334151043</v>
+        <v>0.1132672566371681</v>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="P11" t="n">
         <v>0</v>
@@ -1581,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
@@ -1590,10 +1590,10 @@
         <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W11" t="n">
-        <v>0</v>
+        <v>0.8405345132743363</v>
       </c>
       <c r="X11" t="n">
         <v>0</v>
@@ -1605,7 +1605,7 @@
         <v>0</v>
       </c>
       <c r="AA11" t="n">
-        <v>0</v>
+        <v>0.1593522123893805</v>
       </c>
       <c r="AB11" t="n">
         <v>0</v>
@@ -1614,65 +1614,65 @@
         <v>0</v>
       </c>
       <c r="AD11" t="n">
-        <v>1.000035044681969</v>
+        <v>0</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>1-hexene, 4,5-dimethyl-</t>
+          <t>2-cyclopenten-1-one, 2-methyl-</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4,5-dimethylhex-1-ene</t>
+          <t>2-methylcyclopent-2-en-1-one</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>C8H16</t>
+          <t>C6H8O</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>CC(C)C(C)CC=C</t>
+          <t>CC1=CCCC1=O</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>112.21</v>
+        <v>96.13</v>
       </c>
       <c r="F12" t="n">
-        <v>3.5</v>
+        <v>0.9</v>
       </c>
       <c r="G12" t="n">
+        <v>6</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
         <v>8</v>
       </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>16</v>
-      </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>0.8563229658675697</v>
+        <v>0.7496723187350464</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.1437305053025577</v>
+        <v>0.08388640382814938</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>0.1664308748569645</v>
       </c>
       <c r="O12" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="P12" t="n">
         <v>0</v>
@@ -1693,10 +1693,10 @@
         <v>0</v>
       </c>
       <c r="V12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W12" t="n">
-        <v>1.000053471170127</v>
+        <v>0.4377509622386352</v>
       </c>
       <c r="X12" t="n">
         <v>0</v>
@@ -1717,78 +1717,78 @@
         <v>0</v>
       </c>
       <c r="AD12" t="n">
-        <v>0</v>
+        <v>0.5936960366170811</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>trans-2-pentenoic acid</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>(e)-pent-2-enoic acid</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>C6H6O</t>
+          <t>C5H8O2</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>C1=CC=C(C=C1)O</t>
+          <t>CCC=CC(=O)O</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>94.11</v>
+        <v>100.12</v>
       </c>
       <c r="F13" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J13" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.5998302037554933</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.08054334798242109</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.3195964842189373</v>
+      </c>
+      <c r="O13" t="n">
+        <v>4</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
         <v>1</v>
       </c>
-      <c r="K13" t="n">
-        <v>0.765763468281798</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0.06426522154925088</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.1700031877590054</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" t="n">
-        <v>1</v>
-      </c>
-      <c r="S13" t="n">
-        <v>0</v>
-      </c>
       <c r="T13" t="n">
         <v>0</v>
       </c>
@@ -1799,19 +1799,19 @@
         <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>0</v>
+        <v>0.5503395924890131</v>
       </c>
       <c r="X13" t="n">
-        <v>0.8193178195728402</v>
+        <v>0</v>
       </c>
       <c r="Y13" t="n">
         <v>0</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.1807140580172139</v>
+        <v>0</v>
       </c>
       <c r="AA13" t="n">
-        <v>0</v>
+        <v>0.4496304434678386</v>
       </c>
       <c r="AB13" t="n">
         <v>0</v>
@@ -1823,75 +1823,75 @@
         <v>0</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>2-methylcyclopent-2-en-1-one</t>
+          <t>n-decanoic acid</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2-methylcyclopent-2-en-1-one</t>
+          <t>decanoic acid</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>C6H8O</t>
+          <t>C10H20O2</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>CC1=CCCC1=O</t>
+          <t>CCCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>96.13</v>
+        <v>172.26</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9</v>
+        <v>4.1</v>
       </c>
       <c r="G14" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J14" t="n">
+        <v>2</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.6972599558806455</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.1170323928944619</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.1857540926506444</v>
+      </c>
+      <c r="O14" t="n">
+        <v>9</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
         <v>1</v>
       </c>
-      <c r="K14" t="n">
-        <v>0.7496723187350464</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0.08388640382814938</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0.1664308748569645</v>
-      </c>
-      <c r="O14" t="n">
-        <v>3</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" t="n">
-        <v>0</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0</v>
-      </c>
       <c r="T14" t="n">
         <v>0</v>
       </c>
@@ -1899,10 +1899,10 @@
         <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W14" t="n">
-        <v>0.4377509622386352</v>
+        <v>0.7387147335423198</v>
       </c>
       <c r="X14" t="n">
         <v>0</v>
@@ -1914,7 +1914,7 @@
         <v>0</v>
       </c>
       <c r="AA14" t="n">
-        <v>0</v>
+        <v>0.2613317078834321</v>
       </c>
       <c r="AB14" t="n">
         <v>0</v>
@@ -1923,74 +1923,74 @@
         <v>0</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.5936960366170811</v>
+        <v>0</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>2,4,5-trichlorophenol</t>
+          <t>1-hexene, 4,5-dimethyl-</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2,4,5-trichlorophenol</t>
+          <t>4,5-dimethylhex-1-ene</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>C6H3Cl3O</t>
+          <t>C8H16</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>C1=C(C(=CC(=C1Cl)Cl)Cl)O</t>
+          <t>CC(C)C(C)CC=C</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>197.4</v>
+        <v>112.21</v>
       </c>
       <c r="F15" t="n">
-        <v>3.7</v>
+        <v>3.5</v>
       </c>
       <c r="G15" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="J15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.3650759878419453</v>
+        <v>0.8563229658675697</v>
       </c>
       <c r="L15" t="n">
-        <v>0.5387537993920973</v>
+        <v>0</v>
       </c>
       <c r="M15" t="n">
-        <v>0.01531914893617021</v>
+        <v>0.1437305053025577</v>
       </c>
       <c r="N15" t="n">
-        <v>0.08104863221884498</v>
+        <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P15" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15" t="n">
         <v>0</v>
@@ -1999,22 +1999,22 @@
         <v>0</v>
       </c>
       <c r="U15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V15" t="n">
         <v>0</v>
       </c>
       <c r="W15" t="n">
-        <v>0</v>
+        <v>1.000053471170127</v>
       </c>
       <c r="X15" t="n">
-        <v>0.3752887537993921</v>
+        <v>0</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.5387537993920973</v>
+        <v>0</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.08615501519756839</v>
+        <v>0</v>
       </c>
       <c r="AA15" t="n">
         <v>0</v>
@@ -2023,41 +2023,41 @@
         <v>0</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.5387537993920973</v>
+        <v>0</v>
       </c>
       <c r="AD15" t="n">
         <v>0</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>hexadecanoic acid</t>
+          <t>oxacycloheptadecan-2-one</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>hexadecanoic acid</t>
+          <t>oxacycloheptadecan-2-one</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>C16H32O2</t>
+          <t>C16H30O2</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCCCC(=O)O</t>
+          <t>C1CCCCCCCC(=O)OCCCCCCC1</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>256.42</v>
+        <v>254.41</v>
       </c>
       <c r="F16" t="n">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="G16" t="n">
         <v>16</v>
@@ -2066,25 +2066,25 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J16" t="n">
         <v>2</v>
       </c>
       <c r="K16" t="n">
-        <v>0.7494579205990172</v>
+        <v>0.7553791124562713</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>0.125793619842446</v>
+        <v>0.1188632522306513</v>
       </c>
       <c r="N16" t="n">
-        <v>0.1247874580765931</v>
+        <v>0.1257733579654888</v>
       </c>
       <c r="O16" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
@@ -2096,11 +2096,11 @@
         <v>0</v>
       </c>
       <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
         <v>1</v>
       </c>
-      <c r="T16" t="n">
-        <v>0</v>
-      </c>
       <c r="U16" t="n">
         <v>0</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>0</v>
       </c>
       <c r="W16" t="n">
-        <v>0.8244793697839481</v>
+        <v>0.771895758814512</v>
       </c>
       <c r="X16" t="n">
         <v>0</v>
@@ -2120,10 +2120,10 @@
         <v>0</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.1755596287341081</v>
+        <v>0</v>
       </c>
       <c r="AB16" t="n">
-        <v>0</v>
+        <v>0.2281199638378994</v>
       </c>
       <c r="AC16" t="n">
         <v>0</v>
@@ -2132,38 +2132,38 @@
         <v>0</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
+          <t>hexadecanoic acid</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
+          <t>hexadecanoic acid</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>C18H32O2</t>
+          <t>C16H32O2</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
+          <t>CCCCCCCCCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>280.4</v>
+        <v>256.42</v>
       </c>
       <c r="F17" t="n">
-        <v>6.8</v>
+        <v>6.4</v>
       </c>
       <c r="G17" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -2175,19 +2175,19 @@
         <v>2</v>
       </c>
       <c r="K17" t="n">
-        <v>0.7710342368045648</v>
+        <v>0.7494579205990172</v>
       </c>
       <c r="L17" t="n">
         <v>0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.1150356633380885</v>
+        <v>0.125793619842446</v>
       </c>
       <c r="N17" t="n">
-        <v>0.1141155492154066</v>
+        <v>0.1247874580765931</v>
       </c>
       <c r="O17" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P17" t="n">
         <v>0</v>
@@ -2211,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="W17" t="n">
-        <v>0.8396398002853066</v>
+        <v>0.8244793697839481</v>
       </c>
       <c r="X17" t="n">
         <v>0</v>
@@ -2223,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.1605456490727532</v>
+        <v>0.1755596287341081</v>
       </c>
       <c r="AB17" t="n">
         <v>0</v>
@@ -2235,62 +2235,62 @@
         <v>0</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>(z)-octadec-9-enoic acid</t>
+          <t>n-hexadecanoic acid</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>(z)-octadec-9-enoic acid</t>
+          <t>hexadecanoic acid</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>C18H34O2</t>
+          <t>C16H32O2</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
+          <t>CCCCCCCCCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>282.5</v>
+        <v>256.42</v>
       </c>
       <c r="F18" t="n">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="G18" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J18" t="n">
         <v>2</v>
       </c>
       <c r="K18" t="n">
-        <v>0.7653026548672566</v>
+        <v>0.7494579205990172</v>
       </c>
       <c r="L18" t="n">
         <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>0.121316814159292</v>
+        <v>0.125793619842446</v>
       </c>
       <c r="N18" t="n">
-        <v>0.1132672566371681</v>
+        <v>0.1247874580765931</v>
       </c>
       <c r="O18" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P18" t="n">
         <v>0</v>
@@ -2314,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="W18" t="n">
-        <v>0.8405345132743363</v>
+        <v>0.8244793697839481</v>
       </c>
       <c r="X18" t="n">
         <v>0</v>
@@ -2326,7 +2326,7 @@
         <v>0</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.1593522123893805</v>
+        <v>0.1755596287341081</v>
       </c>
       <c r="AB18" t="n">
         <v>0</v>
@@ -2338,7 +2338,7 @@
         <v>0</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.9998867256637168</v>
+        <v>1.000038998518056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed std issue in samples, for real
</commit_message>
<xml_diff>
--- a/tests/data_for_testing/compounds_properties.xlsx
+++ b/tests/data_for_testing/compounds_properties.xlsx
@@ -593,56 +593,56 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>oleic acid</t>
+          <t>hexadecanoic acid</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(z)-octadec-9-enoic acid</t>
+          <t>hexadecanoic acid</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C18H34O2</t>
+          <t>C16H32O2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
+          <t>CCCCCCCCCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>282.5</v>
+        <v>256.42</v>
       </c>
       <c r="F2" t="n">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="G2" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J2" t="n">
         <v>2</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7653026548672566</v>
+        <v>0.7494579205990172</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.121316814159292</v>
+        <v>0.125793619842446</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1132672566371681</v>
+        <v>0.1247874580765931</v>
       </c>
       <c r="O2" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -666,7 +666,7 @@
         <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>0.8405345132743363</v>
+        <v>0.8244793697839481</v>
       </c>
       <c r="X2" t="n">
         <v>0</v>
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.1593522123893805</v>
+        <v>0.1755596287341081</v>
       </c>
       <c r="AB2" t="n">
         <v>0</v>
@@ -690,62 +690,62 @@
         <v>0</v>
       </c>
       <c r="AE2" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
+          <t>2,5-hexanedione</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
+          <t>hexane-2,5-dione</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C18H32O2</t>
+          <t>C6H10O2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
+          <t>CC(=O)CCC(=O)C</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>280.4</v>
+        <v>114.14</v>
       </c>
       <c r="F3" t="n">
-        <v>6.8</v>
+        <v>-0.3</v>
       </c>
       <c r="G3" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="J3" t="n">
         <v>2</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7710342368045648</v>
+        <v>0.6313825127036973</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.1150356633380885</v>
+        <v>0.08831259856316805</v>
       </c>
       <c r="N3" t="n">
-        <v>0.1141155492154066</v>
+        <v>0.2803399334151043</v>
       </c>
       <c r="O3" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
         <v>0</v>
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
@@ -766,10 +766,10 @@
         <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W3" t="n">
-        <v>0.8396398002853066</v>
+        <v>0</v>
       </c>
       <c r="X3" t="n">
         <v>0</v>
@@ -781,7 +781,7 @@
         <v>0</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.1605456490727532</v>
+        <v>0</v>
       </c>
       <c r="AB3" t="n">
         <v>0</v>
@@ -790,65 +790,65 @@
         <v>0</v>
       </c>
       <c r="AD3" t="n">
-        <v>0</v>
+        <v>1.000035044681969</v>
       </c>
       <c r="AE3" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>2,5-hexanedione</t>
+          <t>trans-2-pentenoic acid</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>hexane-2,5-dione</t>
+          <t>(e)-pent-2-enoic acid</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C6H10O2</t>
+          <t>C5H8O2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CC(=O)CCC(=O)C</t>
+          <t>CCC=CC(=O)O</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>114.14</v>
+        <v>100.12</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.3</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J4" t="n">
         <v>2</v>
       </c>
       <c r="K4" t="n">
-        <v>0.6313825127036973</v>
+        <v>0.5998302037554933</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.08831259856316805</v>
+        <v>0.08054334798242109</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2803399334151043</v>
+        <v>0.3195964842189373</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
@@ -860,7 +860,7 @@
         <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4" t="n">
         <v>0</v>
@@ -869,10 +869,10 @@
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>0</v>
+        <v>0.5503395924890131</v>
       </c>
       <c r="X4" t="n">
         <v>0</v>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="AA4" t="n">
-        <v>0</v>
+        <v>0.4496304434678386</v>
       </c>
       <c r="AB4" t="n">
         <v>0</v>
@@ -893,78 +893,78 @@
         <v>0</v>
       </c>
       <c r="AD4" t="n">
-        <v>1.000035044681969</v>
+        <v>0</v>
       </c>
       <c r="AE4" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>2-methylcyclopent-2-en-1-one</t>
+          <t>9,12-octadecadienoic acid (z,z)-</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2-methylcyclopent-2-en-1-one</t>
+          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>C6H8O</t>
+          <t>C18H32O2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CC1=CCCC1=O</t>
+          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>96.13</v>
+        <v>280.4</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9</v>
+        <v>6.8</v>
       </c>
       <c r="G5" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="J5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.7710342368045648</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.1150356633380885</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.1141155492154066</v>
+      </c>
+      <c r="O5" t="n">
+        <v>17</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
         <v>1</v>
       </c>
-      <c r="K5" t="n">
-        <v>0.7496723187350464</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.08388640382814938</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.1664308748569645</v>
-      </c>
-      <c r="O5" t="n">
-        <v>3</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0</v>
-      </c>
       <c r="T5" t="n">
         <v>0</v>
       </c>
@@ -972,10 +972,10 @@
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>0.4377509622386352</v>
+        <v>0.8396398002853066</v>
       </c>
       <c r="X5" t="n">
         <v>0</v>
@@ -987,7 +987,7 @@
         <v>0</v>
       </c>
       <c r="AA5" t="n">
-        <v>0</v>
+        <v>0.1605456490727532</v>
       </c>
       <c r="AB5" t="n">
         <v>0</v>
@@ -996,98 +996,98 @@
         <v>0</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.5936960366170811</v>
+        <v>0</v>
       </c>
       <c r="AE5" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>2,4,5-trichlorophenol</t>
+          <t>2-cyclopenten-1-one, 2-methyl-</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2,4,5-trichlorophenol</t>
+          <t>2-methylcyclopent-2-en-1-one</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C6H3Cl3O</t>
+          <t>C6H8O</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>C1=C(C(=CC(=C1Cl)Cl)Cl)O</t>
+          <t>CC1=CCCC1=O</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>197.4</v>
+        <v>96.13</v>
       </c>
       <c r="F6" t="n">
-        <v>3.7</v>
+        <v>0.9</v>
       </c>
       <c r="G6" t="n">
         <v>6</v>
       </c>
       <c r="H6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J6" t="n">
         <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3650759878419453</v>
+        <v>0.7496723187350464</v>
       </c>
       <c r="L6" t="n">
-        <v>0.5387537993920973</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.01531914893617021</v>
+        <v>0.08388640382814938</v>
       </c>
       <c r="N6" t="n">
-        <v>0.08104863221884498</v>
+        <v>0.1664308748569645</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P6" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
         <v>1</v>
       </c>
-      <c r="S6" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" t="n">
-        <v>3</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0</v>
-      </c>
       <c r="W6" t="n">
-        <v>0</v>
+        <v>0.4377509622386352</v>
       </c>
       <c r="X6" t="n">
-        <v>0.3752887537993921</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.5387537993920973</v>
+        <v>0</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.08615501519756839</v>
+        <v>0</v>
       </c>
       <c r="AA6" t="n">
         <v>0</v>
@@ -1096,68 +1096,68 @@
         <v>0</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.5387537993920973</v>
+        <v>0</v>
       </c>
       <c r="AD6" t="n">
-        <v>0</v>
+        <v>0.5936960366170811</v>
       </c>
       <c r="AE6" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>9,12-octadecadienoic acid (z,z)-</t>
+          <t>1-hexene, 4,5-dimethyl-</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
+          <t>4,5-dimethylhex-1-ene</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>C18H32O2</t>
+          <t>C8H16</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
+          <t>CC(C)C(C)CC=C</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>280.4</v>
+        <v>112.21</v>
       </c>
       <c r="F7" t="n">
-        <v>6.8</v>
+        <v>3.5</v>
       </c>
       <c r="G7" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="J7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.7710342368045648</v>
+        <v>0.8563229658675697</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1150356633380885</v>
+        <v>0.1437305053025577</v>
       </c>
       <c r="N7" t="n">
-        <v>0.1141155492154066</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
@@ -1169,7 +1169,7 @@
         <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
@@ -1181,7 +1181,7 @@
         <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>0.8396398002853066</v>
+        <v>1.000053471170127</v>
       </c>
       <c r="X7" t="n">
         <v>0</v>
@@ -1193,7 +1193,7 @@
         <v>0</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.1605456490727532</v>
+        <v>0</v>
       </c>
       <c r="AB7" t="n">
         <v>0</v>
@@ -1205,62 +1205,62 @@
         <v>0</v>
       </c>
       <c r="AE7" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>tetradecanoic acid</t>
+          <t>n-hexadecanoic acid</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>tetradecanoic acid</t>
+          <t>hexadecanoic acid</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C14H28O2</t>
+          <t>C16H32O2</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCC(=O)O</t>
+          <t>CCCCCCCCCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>228.37</v>
+        <v>256.42</v>
       </c>
       <c r="F8" t="n">
-        <v>5.3</v>
+        <v>6.4</v>
       </c>
       <c r="G8" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="J8" t="n">
         <v>2</v>
       </c>
       <c r="K8" t="n">
-        <v>0.7363226343214958</v>
+        <v>0.7494579205990172</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.1235889127293427</v>
+        <v>0.125793619842446</v>
       </c>
       <c r="N8" t="n">
-        <v>0.1401147261023777</v>
+        <v>0.1247874580765931</v>
       </c>
       <c r="O8" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P8" t="n">
         <v>0</v>
@@ -1284,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>0.8029031834303979</v>
+        <v>0.8244793697839481</v>
       </c>
       <c r="X8" t="n">
         <v>0</v>
@@ -1296,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.1971230897228183</v>
+        <v>0.1755596287341081</v>
       </c>
       <c r="AB8" t="n">
         <v>0</v>
@@ -1308,59 +1308,59 @@
         <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>2,4,5-trichlorophenol</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>2,4,5-trichlorophenol</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>C6H6O</t>
+          <t>C6H3Cl3O</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>C1=CC=C(C=C1)O</t>
+          <t>C1=C(C(=CC(=C1Cl)Cl)Cl)O</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>94.11</v>
+        <v>197.4</v>
       </c>
       <c r="F9" t="n">
-        <v>1.5</v>
+        <v>3.7</v>
       </c>
       <c r="G9" t="n">
         <v>6</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I9" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J9" t="n">
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>0.765763468281798</v>
+        <v>0.3650759878419453</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>0.5387537993920973</v>
       </c>
       <c r="M9" t="n">
-        <v>0.06426522154925088</v>
+        <v>0.01531914893617021</v>
       </c>
       <c r="N9" t="n">
-        <v>0.1700031877590054</v>
+        <v>0.08104863221884498</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
@@ -1369,7 +1369,7 @@
         <v>6</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R9" t="n">
         <v>1</v>
@@ -1381,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V9" t="n">
         <v>0</v>
@@ -1390,13 +1390,13 @@
         <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>0.8193178195728402</v>
+        <v>0.3752887537993921</v>
       </c>
       <c r="Y9" t="n">
-        <v>0</v>
+        <v>0.5387537993920973</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.1807140580172139</v>
+        <v>0.08615501519756839</v>
       </c>
       <c r="AA9" t="n">
         <v>0</v>
@@ -1405,81 +1405,81 @@
         <v>0</v>
       </c>
       <c r="AC9" t="n">
-        <v>0</v>
+        <v>0.5387537993920973</v>
       </c>
       <c r="AD9" t="n">
         <v>0</v>
       </c>
       <c r="AE9" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>2-butanone</t>
+          <t>(z)-octadec-9-enoic acid</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>butan-2-one</t>
+          <t>(z)-octadec-9-enoic acid</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>C4H8O</t>
+          <t>C18H34O2</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>CCC(=O)C</t>
+          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>72.11</v>
+        <v>282.5</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3</v>
+        <v>6.5</v>
       </c>
       <c r="G10" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="J10" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.7653026548672566</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.121316814159292</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.1132672566371681</v>
+      </c>
+      <c r="O10" t="n">
+        <v>17</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
         <v>1</v>
       </c>
-      <c r="K10" t="n">
-        <v>0.6662598807377618</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.1118291499098599</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.2218693662460131</v>
-      </c>
-      <c r="O10" t="n">
-        <v>1</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" t="n">
-        <v>0</v>
-      </c>
       <c r="T10" t="n">
         <v>0</v>
       </c>
@@ -1487,10 +1487,10 @@
         <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>0.2085009014006379</v>
+        <v>0.8405345132743363</v>
       </c>
       <c r="X10" t="n">
         <v>0</v>
@@ -1502,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="AA10" t="n">
-        <v>0</v>
+        <v>0.1593522123893805</v>
       </c>
       <c r="AB10" t="n">
         <v>0</v>
@@ -1511,65 +1511,65 @@
         <v>0</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.7914574954929968</v>
+        <v>0</v>
       </c>
       <c r="AE10" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>(z)-octadec-9-enoic acid</t>
+          <t>tetradecanoic acid</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>(z)-octadec-9-enoic acid</t>
+          <t>tetradecanoic acid</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>C18H34O2</t>
+          <t>C14H28O2</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
+          <t>CCCCCCCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>282.5</v>
+        <v>228.37</v>
       </c>
       <c r="F11" t="n">
-        <v>6.5</v>
+        <v>5.3</v>
       </c>
       <c r="G11" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J11" t="n">
         <v>2</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7653026548672566</v>
+        <v>0.7363226343214958</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>0.121316814159292</v>
+        <v>0.1235889127293427</v>
       </c>
       <c r="N11" t="n">
-        <v>0.1132672566371681</v>
+        <v>0.1401147261023777</v>
       </c>
       <c r="O11" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="P11" t="n">
         <v>0</v>
@@ -1593,7 +1593,7 @@
         <v>0</v>
       </c>
       <c r="W11" t="n">
-        <v>0.8405345132743363</v>
+        <v>0.8029031834303979</v>
       </c>
       <c r="X11" t="n">
         <v>0</v>
@@ -1605,7 +1605,7 @@
         <v>0</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.1593522123893805</v>
+        <v>0.1971230897228183</v>
       </c>
       <c r="AB11" t="n">
         <v>0</v>
@@ -1617,38 +1617,38 @@
         <v>0</v>
       </c>
       <c r="AE11" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>2-cyclopenten-1-one, 2-methyl-</t>
+          <t>2-butanone</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2-methylcyclopent-2-en-1-one</t>
+          <t>butan-2-one</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>C6H8O</t>
+          <t>C4H8O</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>CC1=CCCC1=O</t>
+          <t>CCC(=O)C</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>96.13</v>
+        <v>72.11</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="G12" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1660,19 +1660,19 @@
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>0.7496723187350464</v>
+        <v>0.6662598807377618</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.08388640382814938</v>
+        <v>0.1118291499098599</v>
       </c>
       <c r="N12" t="n">
-        <v>0.1664308748569645</v>
+        <v>0.2218693662460131</v>
       </c>
       <c r="O12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P12" t="n">
         <v>0</v>
@@ -1696,7 +1696,7 @@
         <v>1</v>
       </c>
       <c r="W12" t="n">
-        <v>0.4377509622386352</v>
+        <v>0.2085009014006379</v>
       </c>
       <c r="X12" t="n">
         <v>0</v>
@@ -1717,65 +1717,65 @@
         <v>0</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.5936960366170811</v>
+        <v>0.7914574954929968</v>
       </c>
       <c r="AE12" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>trans-2-pentenoic acid</t>
+          <t>oleic acid</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>(e)-pent-2-enoic acid</t>
+          <t>(z)-octadec-9-enoic acid</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>C5H8O2</t>
+          <t>C18H34O2</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>CCC=CC(=O)O</t>
+          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>100.12</v>
+        <v>282.5</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>6.5</v>
       </c>
       <c r="G13" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="J13" t="n">
         <v>2</v>
       </c>
       <c r="K13" t="n">
-        <v>0.5998302037554933</v>
+        <v>0.7653026548672566</v>
       </c>
       <c r="L13" t="n">
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>0.08054334798242109</v>
+        <v>0.121316814159292</v>
       </c>
       <c r="N13" t="n">
-        <v>0.3195964842189373</v>
+        <v>0.1132672566371681</v>
       </c>
       <c r="O13" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="P13" t="n">
         <v>0</v>
@@ -1799,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>0.5503395924890131</v>
+        <v>0.8405345132743363</v>
       </c>
       <c r="X13" t="n">
         <v>0</v>
@@ -1811,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.4496304434678386</v>
+        <v>0.1593522123893805</v>
       </c>
       <c r="AB13" t="n">
         <v>0</v>
@@ -1823,7 +1823,7 @@
         <v>0</v>
       </c>
       <c r="AE13" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="14">
@@ -1926,62 +1926,62 @@
         <v>0</v>
       </c>
       <c r="AE14" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>1-hexene, 4,5-dimethyl-</t>
+          <t>2-methylcyclopent-2-en-1-one</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4,5-dimethylhex-1-ene</t>
+          <t>2-methylcyclopent-2-en-1-one</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>C8H16</t>
+          <t>C6H8O</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>CC(C)C(C)CC=C</t>
+          <t>CC1=CCCC1=O</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>112.21</v>
+        <v>96.13</v>
       </c>
       <c r="F15" t="n">
-        <v>3.5</v>
+        <v>0.9</v>
       </c>
       <c r="G15" t="n">
+        <v>6</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
         <v>8</v>
       </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>16</v>
-      </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>0.8563229658675697</v>
+        <v>0.7496723187350464</v>
       </c>
       <c r="L15" t="n">
         <v>0</v>
       </c>
       <c r="M15" t="n">
-        <v>0.1437305053025577</v>
+        <v>0.08388640382814938</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>0.1664308748569645</v>
       </c>
       <c r="O15" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="P15" t="n">
         <v>0</v>
@@ -2002,10 +2002,10 @@
         <v>0</v>
       </c>
       <c r="V15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W15" t="n">
-        <v>1.000053471170127</v>
+        <v>0.4377509622386352</v>
       </c>
       <c r="X15" t="n">
         <v>0</v>
@@ -2026,80 +2026,80 @@
         <v>0</v>
       </c>
       <c r="AD15" t="n">
-        <v>0</v>
+        <v>0.5936960366170811</v>
       </c>
       <c r="AE15" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>oxacycloheptadecan-2-one</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>oxacycloheptadecan-2-one</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>C16H30O2</t>
+          <t>C6H6O</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>C1CCCCCCCC(=O)OCCCCCCC1</t>
+          <t>C1=CC=C(C=C1)O</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>254.41</v>
+        <v>94.11</v>
       </c>
       <c r="F16" t="n">
-        <v>6.3</v>
+        <v>1.5</v>
       </c>
       <c r="G16" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="J16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16" t="n">
-        <v>0.7553791124562713</v>
+        <v>0.765763468281798</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>0.1188632522306513</v>
+        <v>0.06426522154925088</v>
       </c>
       <c r="N16" t="n">
-        <v>0.1257733579654888</v>
+        <v>0.1700031877590054</v>
       </c>
       <c r="O16" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q16" t="n">
         <v>0</v>
       </c>
       <c r="R16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S16" t="n">
         <v>0</v>
       </c>
       <c r="T16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U16" t="n">
         <v>0</v>
@@ -2108,22 +2108,22 @@
         <v>0</v>
       </c>
       <c r="W16" t="n">
-        <v>0.771895758814512</v>
+        <v>0</v>
       </c>
       <c r="X16" t="n">
-        <v>0</v>
+        <v>0.8193178195728402</v>
       </c>
       <c r="Y16" t="n">
         <v>0</v>
       </c>
       <c r="Z16" t="n">
-        <v>0</v>
+        <v>0.1807140580172139</v>
       </c>
       <c r="AA16" t="n">
         <v>0</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.2281199638378994</v>
+        <v>0</v>
       </c>
       <c r="AC16" t="n">
         <v>0</v>
@@ -2132,38 +2132,38 @@
         <v>0</v>
       </c>
       <c r="AE16" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>hexadecanoic acid</t>
+          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>hexadecanoic acid</t>
+          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>C16H32O2</t>
+          <t>C18H32O2</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCCCC(=O)O</t>
+          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>256.42</v>
+        <v>280.4</v>
       </c>
       <c r="F17" t="n">
-        <v>6.4</v>
+        <v>6.8</v>
       </c>
       <c r="G17" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -2175,19 +2175,19 @@
         <v>2</v>
       </c>
       <c r="K17" t="n">
-        <v>0.7494579205990172</v>
+        <v>0.7710342368045648</v>
       </c>
       <c r="L17" t="n">
         <v>0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.125793619842446</v>
+        <v>0.1150356633380885</v>
       </c>
       <c r="N17" t="n">
-        <v>0.1247874580765931</v>
+        <v>0.1141155492154066</v>
       </c>
       <c r="O17" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="P17" t="n">
         <v>0</v>
@@ -2211,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="W17" t="n">
-        <v>0.8244793697839481</v>
+        <v>0.8396398002853066</v>
       </c>
       <c r="X17" t="n">
         <v>0</v>
@@ -2223,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.1755596287341081</v>
+        <v>0.1605456490727532</v>
       </c>
       <c r="AB17" t="n">
         <v>0</v>
@@ -2235,35 +2235,35 @@
         <v>0</v>
       </c>
       <c r="AE17" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>n-hexadecanoic acid</t>
+          <t>oxacycloheptadecan-2-one</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>hexadecanoic acid</t>
+          <t>oxacycloheptadecan-2-one</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>C16H32O2</t>
+          <t>C16H30O2</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCCCC(=O)O</t>
+          <t>C1CCCCCCCC(=O)OCCCCCCC1</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>256.42</v>
+        <v>254.41</v>
       </c>
       <c r="F18" t="n">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="G18" t="n">
         <v>16</v>
@@ -2272,25 +2272,25 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J18" t="n">
         <v>2</v>
       </c>
       <c r="K18" t="n">
-        <v>0.7494579205990172</v>
+        <v>0.7553791124562713</v>
       </c>
       <c r="L18" t="n">
         <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>0.125793619842446</v>
+        <v>0.1188632522306513</v>
       </c>
       <c r="N18" t="n">
-        <v>0.1247874580765931</v>
+        <v>0.1257733579654888</v>
       </c>
       <c r="O18" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P18" t="n">
         <v>0</v>
@@ -2302,11 +2302,11 @@
         <v>0</v>
       </c>
       <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="n">
         <v>1</v>
       </c>
-      <c r="T18" t="n">
-        <v>0</v>
-      </c>
       <c r="U18" t="n">
         <v>0</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="W18" t="n">
-        <v>0.8244793697839481</v>
+        <v>0.771895758814512</v>
       </c>
       <c r="X18" t="n">
         <v>0</v>
@@ -2326,10 +2326,10 @@
         <v>0</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.1755596287341081</v>
+        <v>0</v>
       </c>
       <c r="AB18" t="n">
-        <v>0</v>
+        <v>0.2281199638378994</v>
       </c>
       <c r="AC18" t="n">
         <v>0</v>
@@ -2338,7 +2338,7 @@
         <v>0</v>
       </c>
       <c r="AE18" t="n">
-        <v>1.000038998518056</v>
+        <v>1.000015722652411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finally fixed the std computation and sample aggr
</commit_message>
<xml_diff>
--- a/tests/data_for_testing/compounds_properties.xlsx
+++ b/tests/data_for_testing/compounds_properties.xlsx
@@ -593,56 +593,56 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>2,5-hexanedione</t>
+          <t>oxacycloheptadecan-2-one</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>hexane-2,5-dione</t>
+          <t>oxacycloheptadecan-2-one</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C6H10O2</t>
+          <t>C16H30O2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CC(=O)CCC(=O)C</t>
+          <t>C1CCCCCCCC(=O)OCCCCCCC1</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>114.14</v>
+        <v>254.41</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.3</v>
+        <v>6.3</v>
       </c>
       <c r="G2" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="J2" t="n">
         <v>2</v>
       </c>
       <c r="K2" t="n">
-        <v>0.6313825127036973</v>
+        <v>0.7553791124562713</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.08831259856316805</v>
+        <v>0.1188632522306513</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2803399334151043</v>
+        <v>0.1257733579654888</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -657,16 +657,16 @@
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2" t="n">
         <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>0</v>
+        <v>0.771895758814512</v>
       </c>
       <c r="X2" t="n">
         <v>0</v>
@@ -681,174 +681,174 @@
         <v>0</v>
       </c>
       <c r="AB2" t="n">
-        <v>0</v>
+        <v>0.2281199638378994</v>
       </c>
       <c r="AC2" t="n">
         <v>0</v>
       </c>
       <c r="AD2" t="n">
-        <v>1.000035044681969</v>
+        <v>0</v>
       </c>
       <c r="AE2" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>2,4,5-trichlorophenol</t>
+          <t>n-hexadecanoic acid</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2,4,5-trichlorophenol</t>
+          <t>hexadecanoic acid</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C6H3Cl3O</t>
+          <t>C16H32O2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>C1=C(C(=CC(=C1Cl)Cl)Cl)O</t>
+          <t>CCCCCCCCCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>197.4</v>
+        <v>256.42</v>
       </c>
       <c r="F3" t="n">
-        <v>3.7</v>
+        <v>6.4</v>
       </c>
       <c r="G3" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="J3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.7494579205990172</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.125793619842446</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.1247874580765931</v>
+      </c>
+      <c r="O3" t="n">
+        <v>15</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
         <v>1</v>
       </c>
-      <c r="K3" t="n">
-        <v>0.3650759878419453</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.5387537993920973</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.01531914893617021</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.08104863221884498</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>3</v>
-      </c>
-      <c r="R3" t="n">
-        <v>1</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
       <c r="T3" t="n">
         <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
         <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>0</v>
+        <v>0.8244793697839481</v>
       </c>
       <c r="X3" t="n">
-        <v>0.3752887537993921</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.5387537993920973</v>
+        <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.08615501519756839</v>
+        <v>0</v>
       </c>
       <c r="AA3" t="n">
-        <v>0</v>
+        <v>0.1755596287341081</v>
       </c>
       <c r="AB3" t="n">
         <v>0</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.5387537993920973</v>
+        <v>0</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
       </c>
       <c r="AE3" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>n-decanoic acid</t>
+          <t>tetradecanoic acid</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>decanoic acid</t>
+          <t>tetradecanoic acid</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C10H20O2</t>
+          <t>C14H28O2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CCCCCCCCCC(=O)O</t>
+          <t>CCCCCCCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>172.26</v>
+        <v>228.37</v>
       </c>
       <c r="F4" t="n">
-        <v>4.1</v>
+        <v>5.3</v>
       </c>
       <c r="G4" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J4" t="n">
         <v>2</v>
       </c>
       <c r="K4" t="n">
-        <v>0.6972599558806455</v>
+        <v>0.7363226343214958</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.1170323928944619</v>
+        <v>0.1235889127293427</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1857540926506444</v>
+        <v>0.1401147261023777</v>
       </c>
       <c r="O4" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
@@ -872,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>0.7387147335423198</v>
+        <v>0.8029031834303979</v>
       </c>
       <c r="X4" t="n">
         <v>0</v>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.2613317078834321</v>
+        <v>0.1971230897228183</v>
       </c>
       <c r="AB4" t="n">
         <v>0</v>
@@ -896,72 +896,72 @@
         <v>0</v>
       </c>
       <c r="AE4" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>2-butanone</t>
+          <t>2,4,5-trichlorophenol</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>butan-2-one</t>
+          <t>2,4,5-trichlorophenol</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>C4H8O</t>
+          <t>C6H3Cl3O</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CCC(=O)C</t>
+          <t>C1=C(C(=CC(=C1Cl)Cl)Cl)O</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>72.11</v>
+        <v>197.4</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3</v>
+        <v>3.7</v>
       </c>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I5" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J5" t="n">
         <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>0.6662598807377618</v>
+        <v>0.3650759878419453</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>0.5387537993920973</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1118291499098599</v>
+        <v>0.01531914893617021</v>
       </c>
       <c r="N5" t="n">
-        <v>0.2218693662460131</v>
+        <v>0.08104863221884498</v>
       </c>
       <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>3</v>
+      </c>
+      <c r="R5" t="n">
         <v>1</v>
       </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
       <c r="S5" t="n">
         <v>0</v>
       </c>
@@ -969,22 +969,22 @@
         <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>0.2085009014006379</v>
+        <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>0</v>
+        <v>0.3752887537993921</v>
       </c>
       <c r="Y5" t="n">
-        <v>0</v>
+        <v>0.5387537993920973</v>
       </c>
       <c r="Z5" t="n">
-        <v>0</v>
+        <v>0.08615501519756839</v>
       </c>
       <c r="AA5" t="n">
         <v>0</v>
@@ -993,68 +993,68 @@
         <v>0</v>
       </c>
       <c r="AC5" t="n">
-        <v>0</v>
+        <v>0.5387537993920973</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.7914574954929968</v>
+        <v>0</v>
       </c>
       <c r="AE5" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>trans-2-pentenoic acid</t>
+          <t>oleic acid</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>(e)-pent-2-enoic acid</t>
+          <t>(z)-octadec-9-enoic acid</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C5H8O2</t>
+          <t>C18H34O2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CCC=CC(=O)O</t>
+          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>100.12</v>
+        <v>282.5</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>6.5</v>
       </c>
       <c r="G6" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="J6" t="n">
         <v>2</v>
       </c>
       <c r="K6" t="n">
-        <v>0.5998302037554933</v>
+        <v>0.7653026548672566</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.08054334798242109</v>
+        <v>0.121316814159292</v>
       </c>
       <c r="N6" t="n">
-        <v>0.3195964842189373</v>
+        <v>0.1132672566371681</v>
       </c>
       <c r="O6" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="P6" t="n">
         <v>0</v>
@@ -1078,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>0.5503395924890131</v>
+        <v>0.8405345132743363</v>
       </c>
       <c r="X6" t="n">
         <v>0</v>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.4496304434678386</v>
+        <v>0.1593522123893805</v>
       </c>
       <c r="AB6" t="n">
         <v>0</v>
@@ -1102,62 +1102,62 @@
         <v>0</v>
       </c>
       <c r="AE6" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>1-hexene, 4,5-dimethyl-</t>
+          <t>2-butanone</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4,5-dimethylhex-1-ene</t>
+          <t>butan-2-one</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>C8H16</t>
+          <t>C4H8O</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CC(C)C(C)CC=C</t>
+          <t>CCC(=O)C</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>112.21</v>
+        <v>72.11</v>
       </c>
       <c r="F7" t="n">
-        <v>3.5</v>
+        <v>0.3</v>
       </c>
       <c r="G7" t="n">
+        <v>4</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
         <v>8</v>
       </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>16</v>
-      </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>0.8563229658675697</v>
+        <v>0.6662598807377618</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1437305053025577</v>
+        <v>0.1118291499098599</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>0.2218693662460131</v>
       </c>
       <c r="O7" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
@@ -1178,10 +1178,10 @@
         <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" t="n">
-        <v>1.000053471170127</v>
+        <v>0.2085009014006379</v>
       </c>
       <c r="X7" t="n">
         <v>0</v>
@@ -1202,38 +1202,38 @@
         <v>0</v>
       </c>
       <c r="AD7" t="n">
-        <v>0</v>
+        <v>0.7914574954929968</v>
       </c>
       <c r="AE7" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>2-cyclopenten-1-one, 2-methyl-</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>phenol</t>
+          <t>2-methylcyclopent-2-en-1-one</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C6H6O</t>
+          <t>C6H8O</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>C1=CC=C(C=C1)O</t>
+          <t>CC1=CCCC1=O</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>94.11</v>
+        <v>96.13</v>
       </c>
       <c r="F8" t="n">
-        <v>1.5</v>
+        <v>0.9</v>
       </c>
       <c r="G8" t="n">
         <v>6</v>
@@ -1242,58 +1242,58 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J8" t="n">
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>0.765763468281798</v>
+        <v>0.7496723187350464</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.06426522154925088</v>
+        <v>0.08388640382814938</v>
       </c>
       <c r="N8" t="n">
-        <v>0.1700031877590054</v>
+        <v>0.1664308748569645</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P8" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
         <v>0</v>
       </c>
       <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
         <v>1</v>
       </c>
-      <c r="S8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T8" t="n">
-        <v>0</v>
-      </c>
-      <c r="U8" t="n">
-        <v>0</v>
-      </c>
-      <c r="V8" t="n">
-        <v>0</v>
-      </c>
       <c r="W8" t="n">
-        <v>0</v>
+        <v>0.4377509622386352</v>
       </c>
       <c r="X8" t="n">
-        <v>0.8193178195728402</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="n">
         <v>0</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.1807140580172139</v>
+        <v>0</v>
       </c>
       <c r="AA8" t="n">
         <v>0</v>
@@ -1305,65 +1305,65 @@
         <v>0</v>
       </c>
       <c r="AD8" t="n">
-        <v>0</v>
+        <v>0.5936960366170811</v>
       </c>
       <c r="AE8" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>oxacycloheptadecan-2-one</t>
+          <t>2-methylcyclopent-2-en-1-one</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>oxacycloheptadecan-2-one</t>
+          <t>2-methylcyclopent-2-en-1-one</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>C16H30O2</t>
+          <t>C6H8O</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>C1CCCCCCCC(=O)OCCCCCCC1</t>
+          <t>CC1=CCCC1=O</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>254.41</v>
+        <v>96.13</v>
       </c>
       <c r="F9" t="n">
-        <v>6.3</v>
+        <v>0.9</v>
       </c>
       <c r="G9" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="J9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>0.7553791124562713</v>
+        <v>0.7496723187350464</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.1188632522306513</v>
+        <v>0.08388640382814938</v>
       </c>
       <c r="N9" t="n">
-        <v>0.1257733579654888</v>
+        <v>0.1664308748569645</v>
       </c>
       <c r="O9" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="P9" t="n">
         <v>0</v>
@@ -1378,16 +1378,16 @@
         <v>0</v>
       </c>
       <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="n">
         <v>1</v>
       </c>
-      <c r="U9" t="n">
-        <v>0</v>
-      </c>
-      <c r="V9" t="n">
-        <v>0</v>
-      </c>
       <c r="W9" t="n">
-        <v>0.771895758814512</v>
+        <v>0.4377509622386352</v>
       </c>
       <c r="X9" t="n">
         <v>0</v>
@@ -1402,84 +1402,84 @@
         <v>0</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.2281199638378994</v>
+        <v>0</v>
       </c>
       <c r="AC9" t="n">
         <v>0</v>
       </c>
       <c r="AD9" t="n">
-        <v>0</v>
+        <v>0.5936960366170811</v>
       </c>
       <c r="AE9" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>2-methylcyclopent-2-en-1-one</t>
+          <t>(z)-octadec-9-enoic acid</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2-methylcyclopent-2-en-1-one</t>
+          <t>(z)-octadec-9-enoic acid</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>C6H8O</t>
+          <t>C18H34O2</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>CC1=CCCC1=O</t>
+          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>96.13</v>
+        <v>282.5</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9</v>
+        <v>6.5</v>
       </c>
       <c r="G10" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="J10" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.7653026548672566</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.121316814159292</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.1132672566371681</v>
+      </c>
+      <c r="O10" t="n">
+        <v>17</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
         <v>1</v>
       </c>
-      <c r="K10" t="n">
-        <v>0.7496723187350464</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.08388640382814938</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.1664308748569645</v>
-      </c>
-      <c r="O10" t="n">
-        <v>3</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" t="n">
-        <v>0</v>
-      </c>
       <c r="T10" t="n">
         <v>0</v>
       </c>
@@ -1487,10 +1487,10 @@
         <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>0.4377509622386352</v>
+        <v>0.8405345132743363</v>
       </c>
       <c r="X10" t="n">
         <v>0</v>
@@ -1502,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="AA10" t="n">
-        <v>0</v>
+        <v>0.1593522123893805</v>
       </c>
       <c r="AB10" t="n">
         <v>0</v>
@@ -1511,65 +1511,65 @@
         <v>0</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.5936960366170811</v>
+        <v>0</v>
       </c>
       <c r="AE10" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
+          <t>2,5-hexanedione</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
+          <t>hexane-2,5-dione</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>C18H32O2</t>
+          <t>C6H10O2</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
+          <t>CC(=O)CCC(=O)C</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>280.4</v>
+        <v>114.14</v>
       </c>
       <c r="F11" t="n">
-        <v>6.8</v>
+        <v>-0.3</v>
       </c>
       <c r="G11" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="J11" t="n">
         <v>2</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7710342368045648</v>
+        <v>0.6313825127036973</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>0.1150356633380885</v>
+        <v>0.08831259856316805</v>
       </c>
       <c r="N11" t="n">
-        <v>0.1141155492154066</v>
+        <v>0.2803399334151043</v>
       </c>
       <c r="O11" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="P11" t="n">
         <v>0</v>
@@ -1581,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
@@ -1590,10 +1590,10 @@
         <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W11" t="n">
-        <v>0.8396398002853066</v>
+        <v>0</v>
       </c>
       <c r="X11" t="n">
         <v>0</v>
@@ -1605,7 +1605,7 @@
         <v>0</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.1605456490727532</v>
+        <v>0</v>
       </c>
       <c r="AB11" t="n">
         <v>0</v>
@@ -1614,65 +1614,65 @@
         <v>0</v>
       </c>
       <c r="AD11" t="n">
-        <v>0</v>
+        <v>1.000035044681969</v>
       </c>
       <c r="AE11" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>9,12-octadecadienoic acid (z,z)-</t>
+          <t>1-hexene, 4,5-dimethyl-</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
+          <t>4,5-dimethylhex-1-ene</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>C18H32O2</t>
+          <t>C8H16</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
+          <t>CC(C)C(C)CC=C</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>280.4</v>
+        <v>112.21</v>
       </c>
       <c r="F12" t="n">
-        <v>6.8</v>
+        <v>3.5</v>
       </c>
       <c r="G12" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="J12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.7710342368045648</v>
+        <v>0.8563229658675697</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.1150356633380885</v>
+        <v>0.1437305053025577</v>
       </c>
       <c r="N12" t="n">
-        <v>0.1141155492154066</v>
+        <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="P12" t="n">
         <v>0</v>
@@ -1684,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="S12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12" t="n">
         <v>0</v>
@@ -1696,7 +1696,7 @@
         <v>0</v>
       </c>
       <c r="W12" t="n">
-        <v>0.8396398002853066</v>
+        <v>1.000053471170127</v>
       </c>
       <c r="X12" t="n">
         <v>0</v>
@@ -1708,7 +1708,7 @@
         <v>0</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.1605456490727532</v>
+        <v>0</v>
       </c>
       <c r="AB12" t="n">
         <v>0</v>
@@ -1720,62 +1720,62 @@
         <v>0</v>
       </c>
       <c r="AE12" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>(z)-octadec-9-enoic acid</t>
+          <t>trans-2-pentenoic acid</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>(z)-octadec-9-enoic acid</t>
+          <t>(e)-pent-2-enoic acid</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>C18H34O2</t>
+          <t>C5H8O2</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
+          <t>CCC=CC(=O)O</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>282.5</v>
+        <v>100.12</v>
       </c>
       <c r="F13" t="n">
-        <v>6.5</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="J13" t="n">
         <v>2</v>
       </c>
       <c r="K13" t="n">
-        <v>0.7653026548672566</v>
+        <v>0.5998302037554933</v>
       </c>
       <c r="L13" t="n">
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>0.121316814159292</v>
+        <v>0.08054334798242109</v>
       </c>
       <c r="N13" t="n">
-        <v>0.1132672566371681</v>
+        <v>0.3195964842189373</v>
       </c>
       <c r="O13" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="P13" t="n">
         <v>0</v>
@@ -1799,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>0.8405345132743363</v>
+        <v>0.5503395924890131</v>
       </c>
       <c r="X13" t="n">
         <v>0</v>
@@ -1811,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.1593522123893805</v>
+        <v>0.4496304434678386</v>
       </c>
       <c r="AB13" t="n">
         <v>0</v>
@@ -1823,62 +1823,62 @@
         <v>0</v>
       </c>
       <c r="AE13" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>n-hexadecanoic acid</t>
+          <t>n-decanoic acid</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>hexadecanoic acid</t>
+          <t>decanoic acid</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>C16H32O2</t>
+          <t>C10H20O2</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCCCC(=O)O</t>
+          <t>CCCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>256.42</v>
+        <v>172.26</v>
       </c>
       <c r="F14" t="n">
-        <v>6.4</v>
+        <v>4.1</v>
       </c>
       <c r="G14" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="J14" t="n">
         <v>2</v>
       </c>
       <c r="K14" t="n">
-        <v>0.7494579205990172</v>
+        <v>0.6972599558806455</v>
       </c>
       <c r="L14" t="n">
         <v>0</v>
       </c>
       <c r="M14" t="n">
-        <v>0.125793619842446</v>
+        <v>0.1170323928944619</v>
       </c>
       <c r="N14" t="n">
-        <v>0.1247874580765931</v>
+        <v>0.1857540926506444</v>
       </c>
       <c r="O14" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="P14" t="n">
         <v>0</v>
@@ -1902,7 +1902,7 @@
         <v>0</v>
       </c>
       <c r="W14" t="n">
-        <v>0.8244793697839481</v>
+        <v>0.7387147335423198</v>
       </c>
       <c r="X14" t="n">
         <v>0</v>
@@ -1914,7 +1914,7 @@
         <v>0</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.1755596287341081</v>
+        <v>0.2613317078834321</v>
       </c>
       <c r="AB14" t="n">
         <v>0</v>
@@ -1926,7 +1926,7 @@
         <v>0</v>
       </c>
       <c r="AE14" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="15">
@@ -2029,35 +2029,35 @@
         <v>0</v>
       </c>
       <c r="AE15" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>2-cyclopenten-1-one, 2-methyl-</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2-methylcyclopent-2-en-1-one</t>
+          <t>phenol</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>C6H8O</t>
+          <t>C6H6O</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>CC1=CCCC1=O</t>
+          <t>C1=CC=C(C=C1)O</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>96.13</v>
+        <v>94.11</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9</v>
+        <v>1.5</v>
       </c>
       <c r="G16" t="n">
         <v>6</v>
@@ -2066,34 +2066,34 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J16" t="n">
         <v>1</v>
       </c>
       <c r="K16" t="n">
-        <v>0.7496723187350464</v>
+        <v>0.765763468281798</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>0.08388640382814938</v>
+        <v>0.06426522154925088</v>
       </c>
       <c r="N16" t="n">
-        <v>0.1664308748569645</v>
+        <v>0.1700031877590054</v>
       </c>
       <c r="O16" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q16" t="n">
         <v>0</v>
       </c>
       <c r="R16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S16" t="n">
         <v>0</v>
@@ -2105,19 +2105,19 @@
         <v>0</v>
       </c>
       <c r="V16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W16" t="n">
-        <v>0.4377509622386352</v>
+        <v>0</v>
       </c>
       <c r="X16" t="n">
-        <v>0</v>
+        <v>0.8193178195728402</v>
       </c>
       <c r="Y16" t="n">
         <v>0</v>
       </c>
       <c r="Z16" t="n">
-        <v>0</v>
+        <v>0.1807140580172139</v>
       </c>
       <c r="AA16" t="n">
         <v>0</v>
@@ -2129,38 +2129,38 @@
         <v>0</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.5936960366170811</v>
+        <v>0</v>
       </c>
       <c r="AE16" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>oleic acid</t>
+          <t>9,12-octadecadienoic acid (z,z)-</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>(z)-octadec-9-enoic acid</t>
+          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>C18H34O2</t>
+          <t>C18H32O2</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>CCCCCCCCC=CCCCCCCCC(=O)O</t>
+          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>282.5</v>
+        <v>280.4</v>
       </c>
       <c r="F17" t="n">
-        <v>6.5</v>
+        <v>6.8</v>
       </c>
       <c r="G17" t="n">
         <v>18</v>
@@ -2169,22 +2169,22 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J17" t="n">
         <v>2</v>
       </c>
       <c r="K17" t="n">
-        <v>0.7653026548672566</v>
+        <v>0.7710342368045648</v>
       </c>
       <c r="L17" t="n">
         <v>0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.121316814159292</v>
+        <v>0.1150356633380885</v>
       </c>
       <c r="N17" t="n">
-        <v>0.1132672566371681</v>
+        <v>0.1141155492154066</v>
       </c>
       <c r="O17" t="n">
         <v>17</v>
@@ -2211,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="W17" t="n">
-        <v>0.8405345132743363</v>
+        <v>0.8396398002853066</v>
       </c>
       <c r="X17" t="n">
         <v>0</v>
@@ -2223,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.1593522123893805</v>
+        <v>0.1605456490727532</v>
       </c>
       <c r="AB17" t="n">
         <v>0</v>
@@ -2235,62 +2235,62 @@
         <v>0</v>
       </c>
       <c r="AE17" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>tetradecanoic acid</t>
+          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>tetradecanoic acid</t>
+          <t>(9z,12z)-octadeca-9,12-dienoic acid</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>C14H28O2</t>
+          <t>C18H32O2</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>CCCCCCCCCCCCCC(=O)O</t>
+          <t>CCCCCC=CCC=CCCCCCCCC(=O)O</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>228.37</v>
+        <v>280.4</v>
       </c>
       <c r="F18" t="n">
-        <v>5.3</v>
+        <v>6.8</v>
       </c>
       <c r="G18" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="J18" t="n">
         <v>2</v>
       </c>
       <c r="K18" t="n">
-        <v>0.7363226343214958</v>
+        <v>0.7710342368045648</v>
       </c>
       <c r="L18" t="n">
         <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>0.1235889127293427</v>
+        <v>0.1150356633380885</v>
       </c>
       <c r="N18" t="n">
-        <v>0.1401147261023777</v>
+        <v>0.1141155492154066</v>
       </c>
       <c r="O18" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="P18" t="n">
         <v>0</v>
@@ -2314,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="W18" t="n">
-        <v>0.8029031834303979</v>
+        <v>0.8396398002853066</v>
       </c>
       <c r="X18" t="n">
         <v>0</v>
@@ -2326,7 +2326,7 @@
         <v>0</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.1971230897228183</v>
+        <v>0.1605456490727532</v>
       </c>
       <c r="AB18" t="n">
         <v>0</v>
@@ -2338,7 +2338,7 @@
         <v>0</v>
       </c>
       <c r="AE18" t="n">
-        <v>1.000026273153216</v>
+        <v>1.00018544935806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>